<commit_message>
added HMI hardware docs
</commit_message>
<xml_diff>
--- a/Docs/utils.xlsx
+++ b/Docs/utils.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15990" yWindow="0" windowWidth="26535" windowHeight="13020" activeTab="1"/>
+    <workbookView xWindow="17190" yWindow="0" windowWidth="26535" windowHeight="13020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NFCv2 LED driver" sheetId="1" r:id="rId1"/>
     <sheet name="NFCv2 USART1" sheetId="2" r:id="rId2"/>
+    <sheet name="LM43603" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>W</t>
   </si>
@@ -115,6 +116,33 @@
   </si>
   <si>
     <t>round(USARTDIV)</t>
+  </si>
+  <si>
+    <t>VREF</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>VOUT</t>
   </si>
 </sst>
 </file>
@@ -762,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,4 +862,95 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>1.0109999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11">
+        <f>1/(1/B6+1/B7)</f>
+        <v>27.791304347826088</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12">
+        <f>1/(1/B8+1/B9)</f>
+        <v>8.7179487179487172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13">
+        <f>B12/(B11+B12)</f>
+        <v>0.23878737541528236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14">
+        <f>$B$4/B13</f>
+        <v>4.233892173913044</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Correct encoder ticks count for the full rotation
</commit_message>
<xml_diff>
--- a/Docs/utils.xlsx
+++ b/Docs/utils.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\RF2Software\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\RF2Software\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19590" yWindow="0" windowWidth="26535" windowHeight="13020" activeTab="3"/>
+    <workbookView xWindow="21075" yWindow="0" windowWidth="26535" windowHeight="13020" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="NFCv2 LED driver" sheetId="1" r:id="rId1"/>
     <sheet name="NFCv2 USART1" sheetId="2" r:id="rId2"/>
     <sheet name="LM43603" sheetId="3" r:id="rId3"/>
     <sheet name="GenericExcercise" sheetId="4" r:id="rId4"/>
+    <sheet name="Servo" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>W</t>
   </si>
@@ -159,6 +160,15 @@
   </si>
   <si>
     <t>Byte count per exercise</t>
+  </si>
+  <si>
+    <t>rpm @50Hz</t>
+  </si>
+  <si>
+    <t>motor</t>
+  </si>
+  <si>
+    <t>rps @50Hz</t>
   </si>
 </sst>
 </file>
@@ -975,7 +985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1085,4 +1095,39 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="19.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2">
+        <v>1395</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <f>B2/60</f>
+        <v>23.25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>